<commit_message>
for Dockerfile20 and Dockerfile2
</commit_message>
<xml_diff>
--- a/lai/valuationquan/CNIESG300index.xlsx
+++ b/lai/valuationquan/CNIESG300index.xlsx
@@ -400,10 +400,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:H2957"/>
+  <dimension ref="A1:H2972"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2943" workbookViewId="0">
-      <selection activeCell="A2958" sqref="A2958"/>
+    <sheetView tabSelected="1" topLeftCell="A2958" workbookViewId="0">
+      <selection activeCell="A2973" sqref="A2973"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -78834,7 +78834,7 @@
         <v>2545</v>
       </c>
       <c r="F2906">
-        <f t="shared" ref="F2906:F2957" si="44">E2906/1000</f>
+        <f t="shared" ref="F2906:F2972" si="44">E2906/1000</f>
         <v>2.5449999999999999</v>
       </c>
       <c r="G2906">
@@ -80219,6 +80219,411 @@
       </c>
       <c r="H2957">
         <v>98988224</v>
+      </c>
+    </row>
+    <row r="2958" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2958" s="1">
+        <v>44907</v>
+      </c>
+      <c r="B2958">
+        <v>2525.6201171875</v>
+      </c>
+      <c r="C2958">
+        <v>2531.699951171875</v>
+      </c>
+      <c r="D2958">
+        <v>2507.830078125</v>
+      </c>
+      <c r="E2958">
+        <v>2509.909912109375</v>
+      </c>
+      <c r="F2958">
+        <f t="shared" si="44"/>
+        <v>2.5099099121093751</v>
+      </c>
+      <c r="G2958">
+        <v>92648032</v>
+      </c>
+      <c r="H2958">
+        <v>92648032</v>
+      </c>
+    </row>
+    <row r="2959" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2959" s="1">
+        <v>44908</v>
+      </c>
+      <c r="B2959">
+        <v>2509.77001953125</v>
+      </c>
+      <c r="C2959">
+        <v>2515.469970703125</v>
+      </c>
+      <c r="D2959">
+        <v>2499.679931640625</v>
+      </c>
+      <c r="E2959">
+        <v>2504.889892578125</v>
+      </c>
+      <c r="F2959">
+        <f t="shared" si="44"/>
+        <v>2.5048898925781251</v>
+      </c>
+      <c r="G2959">
+        <v>71553072</v>
+      </c>
+      <c r="H2959">
+        <v>71553072</v>
+      </c>
+    </row>
+    <row r="2960" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2960" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B2960">
+        <v>2506.239990234375</v>
+      </c>
+      <c r="C2960">
+        <v>2521.469970703125</v>
+      </c>
+      <c r="D2960">
+        <v>2496.070068359375</v>
+      </c>
+      <c r="E2960">
+        <v>2511.169921875</v>
+      </c>
+      <c r="F2960">
+        <f t="shared" si="44"/>
+        <v>2.5111699218750001</v>
+      </c>
+      <c r="G2960">
+        <v>69756152</v>
+      </c>
+      <c r="H2960">
+        <v>69756152</v>
+      </c>
+    </row>
+    <row r="2961" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2961" s="1">
+        <v>44910</v>
+      </c>
+      <c r="B2961">
+        <v>2511.639892578125</v>
+      </c>
+      <c r="C2961">
+        <v>2517.780029296875</v>
+      </c>
+      <c r="D2961">
+        <v>2490.780029296875</v>
+      </c>
+      <c r="E2961">
+        <v>2507.530029296875</v>
+      </c>
+      <c r="F2961">
+        <f t="shared" si="44"/>
+        <v>2.5075300292968752</v>
+      </c>
+      <c r="G2961">
+        <v>62588264</v>
+      </c>
+      <c r="H2961">
+        <v>62588264</v>
+      </c>
+    </row>
+    <row r="2962" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2962" s="1">
+        <v>44911</v>
+      </c>
+      <c r="B2962">
+        <v>2494.68994140625</v>
+      </c>
+      <c r="C2962">
+        <v>2516.090087890625</v>
+      </c>
+      <c r="D2962">
+        <v>2494.280029296875</v>
+      </c>
+      <c r="E2962">
+        <v>2513.300048828125</v>
+      </c>
+      <c r="F2962">
+        <f t="shared" si="44"/>
+        <v>2.5133000488281252</v>
+      </c>
+      <c r="G2962">
+        <v>70926672</v>
+      </c>
+      <c r="H2962">
+        <v>70926672</v>
+      </c>
+    </row>
+    <row r="2963" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2963" s="1">
+        <v>44914</v>
+      </c>
+      <c r="B2963">
+        <v>2512.22998046875</v>
+      </c>
+      <c r="C2963">
+        <v>2518.830078125</v>
+      </c>
+      <c r="D2963">
+        <v>2465.550048828125</v>
+      </c>
+      <c r="E2963">
+        <v>2475.3701171875</v>
+      </c>
+      <c r="F2963">
+        <f t="shared" si="44"/>
+        <v>2.4753701171875</v>
+      </c>
+      <c r="G2963">
+        <v>72239608</v>
+      </c>
+      <c r="H2963">
+        <v>72239608</v>
+      </c>
+    </row>
+    <row r="2964" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2964" s="1">
+        <v>44915</v>
+      </c>
+      <c r="B2964">
+        <v>2465.81005859375</v>
+      </c>
+      <c r="C2964">
+        <v>2465.81005859375</v>
+      </c>
+      <c r="D2964">
+        <v>2418.570068359375</v>
+      </c>
+      <c r="E2964">
+        <v>2429.0400390625</v>
+      </c>
+      <c r="F2964">
+        <f t="shared" si="44"/>
+        <v>2.4290400390625</v>
+      </c>
+      <c r="G2964">
+        <v>59058248</v>
+      </c>
+      <c r="H2964">
+        <v>59058248</v>
+      </c>
+    </row>
+    <row r="2965" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2965" s="1">
+        <v>44916</v>
+      </c>
+      <c r="B2965">
+        <v>2436.469970703125</v>
+      </c>
+      <c r="C2965">
+        <v>2445.110107421875</v>
+      </c>
+      <c r="D2965">
+        <v>2425.72998046875</v>
+      </c>
+      <c r="E2965">
+        <v>2431.47998046875</v>
+      </c>
+      <c r="F2965">
+        <f t="shared" si="44"/>
+        <v>2.4314799804687501</v>
+      </c>
+      <c r="G2965">
+        <v>45334076</v>
+      </c>
+      <c r="H2965">
+        <v>45334076</v>
+      </c>
+    </row>
+    <row r="2966" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2966" s="1">
+        <v>44917</v>
+      </c>
+      <c r="B2966">
+        <v>2450.360107421875</v>
+      </c>
+      <c r="C2966">
+        <v>2466.93994140625</v>
+      </c>
+      <c r="D2966">
+        <v>2428.5</v>
+      </c>
+      <c r="E2966">
+        <v>2437.219970703125</v>
+      </c>
+      <c r="F2966">
+        <f t="shared" si="44"/>
+        <v>2.4372199707031248</v>
+      </c>
+      <c r="G2966">
+        <v>59593360</v>
+      </c>
+      <c r="H2966">
+        <v>59593360</v>
+      </c>
+    </row>
+    <row r="2967" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2967" s="1">
+        <v>44918</v>
+      </c>
+      <c r="B2967">
+        <v>2422.469970703125</v>
+      </c>
+      <c r="C2967">
+        <v>2447.800048828125</v>
+      </c>
+      <c r="D2967">
+        <v>2419.080078125</v>
+      </c>
+      <c r="E2967">
+        <v>2435.280029296875</v>
+      </c>
+      <c r="F2967">
+        <f t="shared" si="44"/>
+        <v>2.4352800292968748</v>
+      </c>
+      <c r="G2967">
+        <v>44959140</v>
+      </c>
+      <c r="H2967">
+        <v>44959140</v>
+      </c>
+    </row>
+    <row r="2968" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2968" s="1">
+        <v>44921</v>
+      </c>
+      <c r="B2968">
+        <v>2437.3798828125</v>
+      </c>
+      <c r="C2968">
+        <v>2450.10009765625</v>
+      </c>
+      <c r="D2968">
+        <v>2433.010009765625</v>
+      </c>
+      <c r="E2968">
+        <v>2438.929931640625</v>
+      </c>
+      <c r="F2968">
+        <f t="shared" si="44"/>
+        <v>2.438929931640625</v>
+      </c>
+      <c r="G2968">
+        <v>53535068</v>
+      </c>
+      <c r="H2968">
+        <v>53535068</v>
+      </c>
+    </row>
+    <row r="2969" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2969" s="1">
+        <v>44922</v>
+      </c>
+      <c r="B2969">
+        <v>2449.8701171875</v>
+      </c>
+      <c r="C2969">
+        <v>2469.169921875</v>
+      </c>
+      <c r="D2969">
+        <v>2446.93994140625</v>
+      </c>
+      <c r="E2969">
+        <v>2466.10009765625</v>
+      </c>
+      <c r="F2969">
+        <f t="shared" si="44"/>
+        <v>2.4661000976562502</v>
+      </c>
+      <c r="G2969">
+        <v>57878804</v>
+      </c>
+      <c r="H2969">
+        <v>57878804</v>
+      </c>
+    </row>
+    <row r="2970" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2970" s="1">
+        <v>44923</v>
+      </c>
+      <c r="B2970">
+        <v>2460.1201171875</v>
+      </c>
+      <c r="C2970">
+        <v>2468.030029296875</v>
+      </c>
+      <c r="D2970">
+        <v>2447.60009765625</v>
+      </c>
+      <c r="E2970">
+        <v>2460.739990234375</v>
+      </c>
+      <c r="F2970">
+        <f t="shared" si="44"/>
+        <v>2.4607399902343752</v>
+      </c>
+      <c r="G2970">
+        <v>58449664</v>
+      </c>
+      <c r="H2970">
+        <v>58449664</v>
+      </c>
+    </row>
+    <row r="2971" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2971" s="1">
+        <v>44924</v>
+      </c>
+      <c r="B2971">
+        <v>2448.949951171875</v>
+      </c>
+      <c r="C2971">
+        <v>2457.75</v>
+      </c>
+      <c r="D2971">
+        <v>2438.800048828125</v>
+      </c>
+      <c r="E2971">
+        <v>2451.679931640625</v>
+      </c>
+      <c r="F2971">
+        <f t="shared" si="44"/>
+        <v>2.451679931640625</v>
+      </c>
+      <c r="G2971">
+        <v>56904100</v>
+      </c>
+      <c r="H2971">
+        <v>56904100</v>
+      </c>
+    </row>
+    <row r="2972" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2972" s="1">
+        <v>44925</v>
+      </c>
+      <c r="B2972">
+        <v>2461.929931640625</v>
+      </c>
+      <c r="C2972">
+        <v>2472.47998046875</v>
+      </c>
+      <c r="D2972">
+        <v>2459.989990234375</v>
+      </c>
+      <c r="E2972">
+        <v>2462.43994140625</v>
+      </c>
+      <c r="F2972">
+        <f t="shared" si="44"/>
+        <v>2.4624399414062501</v>
+      </c>
+      <c r="G2972">
+        <v>57921352</v>
+      </c>
+      <c r="H2972">
+        <v>57921352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>